<commit_message>
Update: Cambios en consultas por cambio de año
</commit_message>
<xml_diff>
--- a/public/archivos/Vales2022.xlsx
+++ b/public/archivos/Vales2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21960C9-B985-2843-9BBF-A3F41C9AB772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EA3ED0-4FB1-D143-BC7B-2C75EF2FEB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="-17620" windowWidth="27820" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Correo</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>Sexo</t>
+  </si>
+  <si>
+    <t>Fecha de Nacimiento</t>
+  </si>
+  <si>
+    <t>Entidad Nacimiento</t>
+  </si>
+  <si>
+    <t>idMunicipio</t>
+  </si>
+  <si>
+    <t>Numero Localidad</t>
+  </si>
+  <si>
+    <t>CveInegi Localidad</t>
   </si>
 </sst>
 </file>
@@ -477,15 +492,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:AD2"/>
+  <dimension ref="A2:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -523,57 +544,72 @@
         <v>14</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>